<commit_message>
extended patterns and added dataset stats script
</commit_message>
<xml_diff>
--- a/out/Analysis/Dataset_Labelling.xlsx
+++ b/out/Analysis/Dataset_Labelling.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailuc-my.sharepoint.com/personal/wang2ba_ucmail_uc_edu/Documents/group/students/prateek_kharangate/fault_hunter_fall_2023/Labeling/Assembly/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B1114F4-6D94-4971-B3CD-6007C9007519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3598E31-7E60-47D4-85CC-02ADE65FC36A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3456,7 +3456,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="235">
+  <cellXfs count="234">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -3892,9 +3892,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -10402,11 +10399,11 @@
   <sheetData>
     <row r="1" spans="1:33">
       <c r="A1" s="180"/>
-      <c r="B1" s="231" t="s">
+      <c r="B1" s="230" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="232"/>
-      <c r="D1" s="233"/>
+      <c r="C1" s="231"/>
+      <c r="D1" s="232"/>
       <c r="E1" s="158"/>
       <c r="F1" s="158"/>
       <c r="G1" s="158"/>
@@ -10422,21 +10419,21 @@
       <c r="O1" s="185"/>
       <c r="P1" s="205"/>
       <c r="R1" s="151"/>
-      <c r="S1" s="234"/>
-      <c r="T1" s="234"/>
-      <c r="U1" s="234"/>
+      <c r="S1" s="233"/>
+      <c r="T1" s="233"/>
+      <c r="U1" s="233"/>
       <c r="V1" s="151"/>
       <c r="W1" s="151"/>
       <c r="X1" s="151"/>
       <c r="Y1" s="151"/>
       <c r="Z1" s="151"/>
       <c r="AA1" s="151"/>
-      <c r="AB1" s="234"/>
-      <c r="AC1" s="234"/>
-      <c r="AD1" s="234"/>
-      <c r="AE1" s="234"/>
-      <c r="AF1" s="234"/>
-      <c r="AG1" s="234"/>
+      <c r="AB1" s="233"/>
+      <c r="AC1" s="233"/>
+      <c r="AD1" s="233"/>
+      <c r="AE1" s="233"/>
+      <c r="AF1" s="233"/>
+      <c r="AG1" s="233"/>
     </row>
     <row r="2" spans="1:33" s="126" customFormat="1">
       <c r="A2" s="165" t="s">
@@ -19336,25 +19333,25 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" s="180"/>
-      <c r="B1" s="231" t="s">
+      <c r="B1" s="230" t="s">
         <v>266</v>
       </c>
-      <c r="C1" s="232"/>
-      <c r="D1" s="233"/>
+      <c r="C1" s="231"/>
+      <c r="D1" s="232"/>
       <c r="E1" s="154"/>
       <c r="F1" s="158"/>
       <c r="G1" s="158"/>
       <c r="H1" s="158"/>
       <c r="I1" s="196"/>
       <c r="J1" s="151"/>
-      <c r="K1" s="231" t="s">
+      <c r="K1" s="230" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="232"/>
-      <c r="M1" s="232"/>
-      <c r="N1" s="232"/>
-      <c r="O1" s="232"/>
-      <c r="P1" s="233"/>
+      <c r="L1" s="231"/>
+      <c r="M1" s="231"/>
+      <c r="N1" s="231"/>
+      <c r="O1" s="231"/>
+      <c r="P1" s="232"/>
     </row>
     <row r="2" spans="1:24" s="126" customFormat="1">
       <c r="A2" s="165" t="s">
@@ -29119,7 +29116,7 @@
       <c r="M194" s="109" t="s">
         <v>560</v>
       </c>
-      <c r="N194" s="230" t="s">
+      <c r="N194" s="89" t="s">
         <v>561</v>
       </c>
       <c r="P194" s="67" t="b">

</xml_diff>